<commit_message>
EDIT INDEX & BURNDOWN CHART
</commit_message>
<xml_diff>
--- a/BurnDownChart.xlsx
+++ b/BurnDownChart.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>Project</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Task 21.1</t>
+  </si>
+  <si>
+    <t>Task 22.1</t>
   </si>
 </sst>
 </file>
@@ -451,45 +454,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$28:$Q$28</c:f>
+              <c:f>Sheet1!$F$29:$Q$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>82.5</c:v>
+                  <c:v>81.583333333333329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>75</c:v>
+                  <c:v>74.166666666666657</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.5</c:v>
+                  <c:v>66.749999999999986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>59.333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52.5</c:v>
+                  <c:v>51.916666666666657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45</c:v>
+                  <c:v>44.499999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>37.5</c:v>
+                  <c:v>37.083333333333329</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>29.666666666666661</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22.5</c:v>
+                  <c:v>22.249999999999993</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15</c:v>
+                  <c:v>14.833333333333325</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.5</c:v>
+                  <c:v>7.4166666666666581</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>-8.8817841970012523E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -570,7 +573,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$29:$Q$29</c:f>
+              <c:f>Sheet1!$F$30:$Q$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -625,11 +628,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-176610352"/>
-        <c:axId val="-176600016"/>
+        <c:axId val="1917599504"/>
+        <c:axId val="1917600048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-176610352"/>
+        <c:axId val="1917599504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -639,7 +642,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-176600016"/>
+        <c:crossAx val="1917600048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -647,7 +650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-176600016"/>
+        <c:axId val="1917600048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="-176610352"/>
+        <c:crossAx val="1917599504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1001,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50264,7 +50267,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -50276,7 +50279,9 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
+      <c r="P6" s="4">
+        <v>0</v>
+      </c>
       <c r="Q6" s="4">
         <v>4</v>
       </c>
@@ -50290,8 +50295,8 @@
       <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="7">
-        <v>1971</v>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
@@ -50322,7 +50327,7 @@
         <v>38</v>
       </c>
       <c r="C8" s="7">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>16</v>
@@ -50353,7 +50358,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="7">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>17</v>
@@ -50384,7 +50389,7 @@
         <v>38</v>
       </c>
       <c r="C10" s="7">
-        <v>1978</v>
+        <v>1974</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>25</v>
@@ -50415,7 +50420,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="7">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>28</v>
@@ -50446,7 +50451,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="7">
-        <v>1985</v>
+        <v>1982</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>29</v>
@@ -50477,7 +50482,7 @@
         <v>38</v>
       </c>
       <c r="C13" s="7">
-        <v>1989</v>
+        <v>1985</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>30</v>
@@ -50508,7 +50513,7 @@
         <v>38</v>
       </c>
       <c r="C14" s="7">
-        <v>1993</v>
+        <v>1989</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>31</v>
@@ -50539,7 +50544,7 @@
         <v>38</v>
       </c>
       <c r="C15" s="7">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>26</v>
@@ -50570,7 +50575,7 @@
         <v>38</v>
       </c>
       <c r="C16" s="7">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>32</v>
@@ -50601,7 +50606,7 @@
         <v>38</v>
       </c>
       <c r="C17" s="7">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>27</v>
@@ -50632,7 +50637,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="7">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>33</v>
@@ -50663,7 +50668,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="7">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>34</v>
@@ -50694,7 +50699,7 @@
         <v>38</v>
       </c>
       <c r="C20" s="7">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>35</v>
@@ -50725,7 +50730,7 @@
         <v>38</v>
       </c>
       <c r="C21" s="7">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>36</v>
@@ -50756,7 +50761,7 @@
         <v>38</v>
       </c>
       <c r="C22" s="7">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>37</v>
@@ -50787,13 +50792,13 @@
         <v>38</v>
       </c>
       <c r="C23" s="7">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E23" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -50849,13 +50854,13 @@
         <v>38</v>
       </c>
       <c r="C25" s="7">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E25" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -50880,7 +50885,7 @@
         <v>38</v>
       </c>
       <c r="C26" s="7">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>42</v>
@@ -50911,7 +50916,7 @@
         <v>38</v>
       </c>
       <c r="C27" s="7">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>43</v>
@@ -50938,63 +50943,30 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="8" t="s">
-        <v>18</v>
+      <c r="B28" s="3" t="s">
+        <v>38</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
+      <c r="C28" s="7">
+        <v>2013</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="E28" s="4">
-        <f>SUM(E6:E27)</f>
-        <v>90</v>
+        <v>3</v>
       </c>
-      <c r="F28" s="4">
-        <f>E28-$E$28/12</f>
-        <v>82.5</v>
-      </c>
-      <c r="G28" s="4">
-        <f t="shared" ref="F28:Q28" si="0">F28-$E$28/12</f>
-        <v>75</v>
-      </c>
-      <c r="H28" s="4">
-        <f t="shared" si="0"/>
-        <v>67.5</v>
-      </c>
-      <c r="I28" s="4">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="J28" s="4">
-        <f t="shared" si="0"/>
-        <v>52.5</v>
-      </c>
-      <c r="K28" s="4">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="L28" s="4">
-        <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-      <c r="M28" s="4">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="N28" s="4">
-        <f t="shared" si="0"/>
-        <v>22.5</v>
-      </c>
-      <c r="O28" s="4">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="P28" s="4">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-      <c r="Q28" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
@@ -51003,61 +50975,61 @@
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="4">
-        <f>SUM(E6:E27)</f>
-        <v>90</v>
+        <f>SUM(E6:E28)</f>
+        <v>89</v>
       </c>
       <c r="F29" s="4">
-        <f t="shared" ref="F29:Q29" si="1">SUM(F6:F27)</f>
-        <v>0</v>
+        <f>E29-$E$29/12</f>
+        <v>81.583333333333329</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>F29-$E$29/12</f>
+        <v>74.166666666666657</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>G29-$E$29/12</f>
+        <v>66.749999999999986</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>H29-$E$29/12</f>
+        <v>59.333333333333321</v>
       </c>
       <c r="J29" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>I29-$E$29/12</f>
+        <v>51.916666666666657</v>
       </c>
       <c r="K29" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>J29-$E$29/12</f>
+        <v>44.499999999999993</v>
       </c>
       <c r="L29" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>K29-$E$29/12</f>
+        <v>37.083333333333329</v>
       </c>
       <c r="M29" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>L29-$E$29/12</f>
+        <v>29.666666666666661</v>
       </c>
       <c r="N29" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>M29-$E$29/12</f>
+        <v>22.249999999999993</v>
       </c>
       <c r="O29" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>N29-$E$29/12</f>
+        <v>14.833333333333325</v>
       </c>
       <c r="P29" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>O29-$E$29/12</f>
+        <v>7.4166666666666581</v>
       </c>
       <c r="Q29" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f>P29-$E$29/12</f>
+        <v>-8.8817841970012523E-15</v>
       </c>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
@@ -51066,22 +51038,63 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
+      <c r="B30" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="4">
+        <f>SUM(E6:E28)</f>
+        <v>89</v>
+      </c>
+      <c r="F30" s="4">
+        <f>SUM(F6:F28)</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <f>SUM(G6:G28)</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <f>SUM(H6:H28)</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
+        <f>SUM(I6:I28)</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="4">
+        <f>SUM(J6:J28)</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="4">
+        <f>SUM(K6:K28)</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="4">
+        <f>SUM(L6:L28)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="4">
+        <f>SUM(M6:M28)</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="4">
+        <f>SUM(N6:N28)</f>
+        <v>0</v>
+      </c>
+      <c r="O30" s="4">
+        <f>SUM(O6:O28)</f>
+        <v>0</v>
+      </c>
+      <c r="P30" s="4">
+        <f>SUM(P6:P28)</f>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="4">
+        <f>SUM(Q6:Q28)</f>
+        <v>4</v>
+      </c>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
@@ -51779,9 +51792,7 @@
     </row>
   </sheetData>
   <sheetProtection password="EF56" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="4">
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
+  <mergeCells count="2">
     <mergeCell ref="D3:K3"/>
     <mergeCell ref="E1:J1"/>
   </mergeCells>

</xml_diff>